<commit_message>
compexp2, resp to temp scripts; manuscript updates
</commit_message>
<xml_diff>
--- a/data/compexp/comptest2_setup.xlsx
+++ b/data/compexp/comptest2_setup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timet\Documents\projectCSUN\csunThesisRepo\data\compexp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Research\csunThesis\data\compexp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E15BD4-C00D-4193-9F16-ADA3B5A179EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20D3F15-30C9-4B65-AD83-87414D3380A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40500" yWindow="1830" windowWidth="13290" windowHeight="13620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -506,10 +506,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1360,7 +1359,7 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1445,7 @@
         <v>0.91836734693877542</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G9" si="0">15-SUM(E3:F3)</f>
+        <f t="shared" ref="G3:G8" si="0">15-SUM(E3:F3)</f>
         <v>14.081632653061224</v>
       </c>
       <c r="I3" t="s">
@@ -1536,13 +1535,13 @@
         <f t="shared" si="0"/>
         <v>11.746987951807229</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6">
         <v>57.777777777777779</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6">
         <f>SUM(E58:E61)</f>
         <v>20.76923076923077</v>
       </c>
@@ -1778,10 +1777,10 @@
         <f t="shared" si="1"/>
         <v>12.378640776699029</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15">
         <v>188.88888888888889</v>
       </c>
       <c r="K15" s="1"/>

</xml_diff>